<commit_message>
changed excel, added test link docs
</commit_message>
<xml_diff>
--- a/Docs/Lab2/Lab02_BBT_TCs_Form.xlsx
+++ b/Docs/Lab2/Lab02_BBT_TCs_Form.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C3E63F-223B-4E1B-A7BE-B6213E829A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F2D777-1595-41C0-8D6E-B56164EE8233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="503" yWindow="1388" windowWidth="16199" windowHeight="9397" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -125,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="125">
   <si>
     <t>Informaţiile vor fi preluate din fişiere text.</t>
   </si>
@@ -642,6 +642,12 @@
       </rPr>
       <t xml:space="preserve"> adăugarea unui payment nou (titlu, regizor, an aparitie, actori, categorie, cuvinte cheie);</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Cash </t>
+  </si>
+  <si>
+    <t>TC5_BVA</t>
   </si>
 </sst>
 </file>
@@ -1275,7 +1281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1423,73 +1429,85 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1498,98 +1516,89 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1938,16 +1947,16 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="4" max="4" width="22.5546875" customWidth="1"/>
-    <col min="9" max="9" width="32.88671875" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" customWidth="1"/>
-    <col min="12" max="12" width="12.21875" customWidth="1"/>
+    <col min="4" max="4" width="22.53125" customWidth="1"/>
+    <col min="9" max="9" width="32.86328125" customWidth="1"/>
+    <col min="10" max="10" width="10.53125" customWidth="1"/>
+    <col min="12" max="12" width="12.19921875" customWidth="1"/>
     <col min="14" max="14" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.45">
       <c r="C1" s="57" t="s">
         <v>64</v>
       </c>
@@ -1960,14 +1969,14 @@
       <c r="I1" s="42"/>
       <c r="J1" s="42"/>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.45">
       <c r="H2" s="60" t="s">
         <v>55</v>
       </c>
       <c r="I2" s="60"/>
       <c r="J2" s="60"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.45">
       <c r="H3" s="2"/>
       <c r="I3" s="2" t="s">
         <v>62</v>
@@ -1976,7 +1985,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.45">
       <c r="H4" s="2" t="s">
         <v>57</v>
       </c>
@@ -1987,7 +1996,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.45">
       <c r="H5" s="2" t="s">
         <v>58</v>
       </c>
@@ -1998,7 +2007,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B6" s="30"/>
       <c r="H6" s="2" t="s">
         <v>59</v>
@@ -2006,40 +2015,40 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B8" s="40" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B9" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B10" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B11" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
         <v>115</v>
       </c>
@@ -2047,7 +2056,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
         <v>36</v>
       </c>
@@ -2055,7 +2064,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
         <v>72</v>
       </c>
@@ -2063,32 +2072,32 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B18" s="40" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B19" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
       <c r="C20" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B21" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B22" s="1" t="s">
         <v>51</v>
       </c>
@@ -2105,7 +2114,7 @@
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B23" s="1" t="s">
         <v>63</v>
       </c>
@@ -2122,7 +2131,7 @@
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="39"/>
       <c r="B24" s="56" t="s">
         <v>60</v>
@@ -2140,7 +2149,7 @@
       <c r="M24" s="56"/>
       <c r="N24" s="56"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
       <c r="C26" s="41"/>
     </row>
   </sheetData>
@@ -2161,26 +2170,26 @@
   </sheetPr>
   <dimension ref="B1:M24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.88671875" customWidth="1"/>
+    <col min="2" max="2" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.86328125" customWidth="1"/>
     <col min="7" max="7" width="8" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.796875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.44140625" customWidth="1"/>
+    <col min="10" max="10" width="25.53125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.46484375" customWidth="1"/>
     <col min="13" max="13" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B1" s="57" t="s">
         <v>64</v>
       </c>
@@ -2188,34 +2197,34 @@
       <c r="D1" s="58"/>
       <c r="E1" s="59"/>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B3" s="61" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="83"/>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="68" t="s">
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="63"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B5" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="G5" s="69" t="s">
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="G5" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="69"/>
-      <c r="K5" s="69"/>
-      <c r="L5" s="69"/>
-      <c r="M5" s="69"/>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="73"/>
+      <c r="L5" s="73"/>
+      <c r="M5" s="73"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B6" s="17" t="s">
         <v>5</v>
       </c>
@@ -2228,35 +2237,35 @@
       <c r="E6" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="72" t="s">
+      <c r="G6" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="78" t="s">
+      <c r="H6" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="70" t="s">
+      <c r="I6" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="71"/>
-      <c r="K6" s="71"/>
-      <c r="L6" s="80" t="s">
+      <c r="J6" s="75"/>
+      <c r="K6" s="75"/>
+      <c r="L6" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="80"/>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="M6" s="69"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C7" s="61" t="s">
+      <c r="C7" s="79" t="s">
         <v>73</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>73</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="79"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="68"/>
       <c r="I7" s="17" t="s">
         <v>86</v>
       </c>
@@ -2266,16 +2275,16 @@
       <c r="K7" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="L7" s="70" t="s">
+      <c r="L7" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="M7" s="74"/>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="M7" s="78"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B8" s="4">
         <v>2</v>
       </c>
-      <c r="C8" s="62"/>
+      <c r="C8" s="81"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
         <v>74</v>
@@ -2295,16 +2304,16 @@
       <c r="K8" s="2">
         <v>1</v>
       </c>
-      <c r="L8" s="76" t="s">
+      <c r="L8" s="65" t="s">
         <v>89</v>
       </c>
-      <c r="M8" s="77"/>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="M8" s="66"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B9" s="4">
         <v>3</v>
       </c>
-      <c r="C9" s="61" t="s">
+      <c r="C9" s="79" t="s">
         <v>84</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -2326,16 +2335,16 @@
       <c r="K9" s="2">
         <v>2.5</v>
       </c>
-      <c r="L9" s="76" t="s">
+      <c r="L9" s="65" t="s">
         <v>92</v>
       </c>
-      <c r="M9" s="77"/>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="M9" s="66"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B10" s="4">
         <v>4</v>
       </c>
-      <c r="C10" s="63"/>
+      <c r="C10" s="80"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
         <v>75</v>
@@ -2347,7 +2356,7 @@
         <v>93</v>
       </c>
       <c r="I10" s="2">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>88</v>
@@ -2360,11 +2369,11 @@
       </c>
       <c r="M10" s="45"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B11" s="4">
         <v>5</v>
       </c>
-      <c r="C11" s="62"/>
+      <c r="C11" s="81"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
         <v>76</v>
@@ -2384,16 +2393,16 @@
       <c r="K11" s="28">
         <v>10.35</v>
       </c>
-      <c r="L11" s="66" t="s">
+      <c r="L11" s="70" t="s">
         <v>119</v>
       </c>
-      <c r="M11" s="67"/>
-    </row>
-    <row r="12" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M11" s="71"/>
+    </row>
+    <row r="12" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="4">
         <v>6</v>
       </c>
-      <c r="C12" s="61" t="s">
+      <c r="C12" s="79" t="s">
         <v>78</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -2405,14 +2414,14 @@
       <c r="I12" s="28"/>
       <c r="J12" s="28"/>
       <c r="K12" s="28"/>
-      <c r="L12" s="66"/>
-      <c r="M12" s="67"/>
-    </row>
-    <row r="13" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L12" s="70"/>
+      <c r="M12" s="71"/>
+    </row>
+    <row r="13" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="4">
         <v>7</v>
       </c>
-      <c r="C13" s="63"/>
+      <c r="C13" s="80"/>
       <c r="D13" s="4" t="s">
         <v>80</v>
       </c>
@@ -2425,11 +2434,11 @@
       <c r="L13" s="46"/>
       <c r="M13" s="47"/>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B14" s="4">
         <v>8</v>
       </c>
-      <c r="C14" s="62"/>
+      <c r="C14" s="81"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
         <v>81</v>
@@ -2439,14 +2448,14 @@
       <c r="I14" s="28"/>
       <c r="J14" s="28"/>
       <c r="K14" s="28"/>
-      <c r="L14" s="66"/>
-      <c r="M14" s="67"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="L14" s="70"/>
+      <c r="M14" s="71"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B15" s="4">
         <v>9</v>
       </c>
-      <c r="C15" s="61" t="s">
+      <c r="C15" s="79" t="s">
         <v>82</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -2458,14 +2467,14 @@
       <c r="I15" s="28"/>
       <c r="J15" s="28"/>
       <c r="K15" s="28"/>
-      <c r="L15" s="66"/>
-      <c r="M15" s="67"/>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="L15" s="70"/>
+      <c r="M15" s="71"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B16" s="4">
         <v>10</v>
       </c>
-      <c r="C16" s="62"/>
+      <c r="C16" s="81"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
         <v>83</v>
@@ -2475,14 +2484,14 @@
       <c r="I16" s="28"/>
       <c r="J16" s="28"/>
       <c r="K16" s="28"/>
-      <c r="L16" s="66"/>
-      <c r="M16" s="67"/>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="L16" s="70"/>
+      <c r="M16" s="71"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B17" s="4">
         <v>11</v>
       </c>
-      <c r="C17" s="61" t="s">
+      <c r="C17" s="79" t="s">
         <v>97</v>
       </c>
       <c r="D17" s="4" t="s">
@@ -2494,14 +2503,14 @@
       <c r="I17" s="28"/>
       <c r="J17" s="28"/>
       <c r="K17" s="28"/>
-      <c r="L17" s="66"/>
-      <c r="M17" s="67"/>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="L17" s="70"/>
+      <c r="M17" s="71"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B18" s="4">
         <v>12</v>
       </c>
-      <c r="C18" s="62"/>
+      <c r="C18" s="81"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4" t="s">
         <v>85</v>
@@ -2511,14 +2520,14 @@
       <c r="I18" s="28"/>
       <c r="J18" s="28"/>
       <c r="K18" s="28"/>
-      <c r="L18" s="66"/>
-      <c r="M18" s="67"/>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="L18" s="70"/>
+      <c r="M18" s="71"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B19" s="4">
         <v>13</v>
       </c>
-      <c r="C19" s="61" t="s">
+      <c r="C19" s="79" t="s">
         <v>4</v>
       </c>
       <c r="D19" s="4"/>
@@ -2528,14 +2537,14 @@
       <c r="I19" s="28"/>
       <c r="J19" s="28"/>
       <c r="K19" s="28"/>
-      <c r="L19" s="66"/>
-      <c r="M19" s="67"/>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="L19" s="70"/>
+      <c r="M19" s="71"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B20" s="4">
         <v>14</v>
       </c>
-      <c r="C20" s="62"/>
+      <c r="C20" s="81"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="G20" s="50"/>
@@ -2543,14 +2552,14 @@
       <c r="I20" s="28"/>
       <c r="J20" s="28"/>
       <c r="K20" s="28"/>
-      <c r="L20" s="66"/>
-      <c r="M20" s="67"/>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="L20" s="70"/>
+      <c r="M20" s="71"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B21" s="4">
         <v>15</v>
       </c>
-      <c r="C21" s="61" t="s">
+      <c r="C21" s="79" t="s">
         <v>4</v>
       </c>
       <c r="D21" s="4"/>
@@ -2560,31 +2569,44 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
-      <c r="L21" s="64"/>
-      <c r="M21" s="65"/>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="L21" s="82"/>
+      <c r="M21" s="83"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B22" s="4">
         <v>16</v>
       </c>
-      <c r="C22" s="62"/>
+      <c r="C22" s="81"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.45">
       <c r="G23" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.45">
       <c r="D24" t="s">
         <v>21</v>
       </c>
-      <c r="F24" s="75"/>
-      <c r="G24" s="75"/>
+      <c r="F24" s="64"/>
+      <c r="G24" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C12:C14"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="F24:G24"/>
@@ -2601,19 +2623,6 @@
     <mergeCell ref="G5:M5"/>
     <mergeCell ref="I6:K6"/>
     <mergeCell ref="G6:G7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C12:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2627,28 +2636,28 @@
   </sheetPr>
   <dimension ref="B1:P30"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="B12" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.1328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" customWidth="1"/>
-    <col min="6" max="6" width="5.5546875" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" customWidth="1"/>
+    <col min="6" max="6" width="5.53125" customWidth="1"/>
+    <col min="7" max="7" width="9.46484375" customWidth="1"/>
     <col min="9" max="9" width="10" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5546875" customWidth="1"/>
+    <col min="10" max="10" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.53125" customWidth="1"/>
     <col min="12" max="12" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="23.33203125" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" customWidth="1"/>
+    <col min="15" max="15" width="9.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B1" s="57" t="s">
         <v>64</v>
       </c>
@@ -2656,36 +2665,36 @@
       <c r="D1" s="58"/>
       <c r="E1" s="59"/>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B3" s="61" t="s">
         <v>122</v>
       </c>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="83"/>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B5" s="89" t="s">
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="63"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B5" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
       <c r="E5" s="3"/>
-      <c r="G5" s="69" t="s">
+      <c r="G5" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="69"/>
-      <c r="K5" s="69"/>
-      <c r="L5" s="69"/>
-      <c r="M5" s="69"/>
-      <c r="N5" s="69"/>
-      <c r="O5" s="69"/>
-    </row>
-    <row r="6" spans="2:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="73"/>
+      <c r="L5" s="73"/>
+      <c r="M5" s="73"/>
+      <c r="N5" s="73"/>
+      <c r="O5" s="73"/>
+    </row>
+    <row r="6" spans="2:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
@@ -2696,42 +2705,42 @@
         <v>13</v>
       </c>
       <c r="E6" s="7"/>
-      <c r="G6" s="72" t="s">
+      <c r="G6" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="72" t="s">
+      <c r="H6" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="72" t="s">
+      <c r="I6" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="78" t="s">
+      <c r="J6" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="86" t="s">
+      <c r="K6" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="L6" s="87"/>
-      <c r="M6" s="87"/>
-      <c r="N6" s="86" t="s">
+      <c r="L6" s="93"/>
+      <c r="M6" s="93"/>
+      <c r="N6" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="O6" s="90"/>
-    </row>
-    <row r="7" spans="2:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B7" s="61">
+      <c r="O6" s="92"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B7" s="79">
         <v>1</v>
       </c>
-      <c r="C7" s="91" t="s">
+      <c r="C7" s="84" t="s">
         <v>96</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="G7" s="73"/>
-      <c r="H7" s="73"/>
-      <c r="I7" s="73"/>
-      <c r="J7" s="79"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="77"/>
+      <c r="J7" s="68"/>
       <c r="K7" s="17" t="s">
         <v>86</v>
       </c>
@@ -2741,14 +2750,14 @@
       <c r="M7" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="N7" s="70" t="s">
+      <c r="N7" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="O7" s="74"/>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B8" s="63"/>
-      <c r="C8" s="92"/>
+      <c r="O7" s="78"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B8" s="80"/>
+      <c r="C8" s="85"/>
       <c r="D8" s="2" t="s">
         <v>100</v>
       </c>
@@ -2767,15 +2776,15 @@
       <c r="K8" s="28"/>
       <c r="L8" s="28"/>
       <c r="M8" s="28"/>
-      <c r="N8" s="66"/>
-      <c r="O8" s="67"/>
+      <c r="N8" s="70"/>
+      <c r="O8" s="71"/>
       <c r="P8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B9" s="63"/>
-      <c r="C9" s="92"/>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B9" s="80"/>
+      <c r="C9" s="85"/>
       <c r="D9" s="2" t="s">
         <v>101</v>
       </c>
@@ -2794,14 +2803,14 @@
       <c r="K9" s="52"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
-      <c r="N9" s="84" t="s">
+      <c r="N9" s="88" t="s">
         <v>114</v>
       </c>
-      <c r="O9" s="85"/>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B10" s="63"/>
-      <c r="C10" s="92"/>
+      <c r="O9" s="89"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B10" s="80"/>
+      <c r="C10" s="85"/>
       <c r="D10" s="2" t="s">
         <v>102</v>
       </c>
@@ -2824,14 +2833,14 @@
       <c r="M10" s="28">
         <v>10</v>
       </c>
-      <c r="N10" s="66" t="s">
+      <c r="N10" s="70" t="s">
         <v>89</v>
       </c>
-      <c r="O10" s="67"/>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B11" s="63"/>
-      <c r="C11" s="92"/>
+      <c r="O10" s="71"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B11" s="80"/>
+      <c r="C11" s="85"/>
       <c r="D11" s="2" t="s">
         <v>103</v>
       </c>
@@ -2850,34 +2859,46 @@
       <c r="K11" s="27"/>
       <c r="L11" s="28"/>
       <c r="M11" s="28"/>
-      <c r="N11" s="84" t="s">
+      <c r="N11" s="88" t="s">
         <v>114</v>
       </c>
-      <c r="O11" s="67"/>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B12" s="62"/>
-      <c r="C12" s="93"/>
+      <c r="O11" s="71"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B12" s="81"/>
+      <c r="C12" s="86"/>
       <c r="D12" s="2" t="s">
         <v>104</v>
       </c>
       <c r="G12" s="17">
         <v>5</v>
       </c>
-      <c r="H12" s="12"/>
+      <c r="H12" s="12">
+        <v>4</v>
+      </c>
       <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="66"/>
-      <c r="O12" s="67"/>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B13" s="61">
+      <c r="J12" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="K12" s="27">
+        <v>1000</v>
+      </c>
+      <c r="L12" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="M12" s="28">
+        <v>10</v>
+      </c>
+      <c r="N12" s="70" t="s">
+        <v>89</v>
+      </c>
+      <c r="O12" s="71"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B13" s="79">
         <v>2</v>
       </c>
-      <c r="C13" s="91" t="s">
+      <c r="C13" s="84" t="s">
         <v>98</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -2892,12 +2913,12 @@
       <c r="K13" s="16"/>
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
-      <c r="N13" s="84"/>
-      <c r="O13" s="85"/>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B14" s="63"/>
-      <c r="C14" s="92"/>
+      <c r="N13" s="88"/>
+      <c r="O13" s="89"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B14" s="80"/>
+      <c r="C14" s="85"/>
       <c r="D14" s="2" t="s">
         <v>107</v>
       </c>
@@ -2910,12 +2931,12 @@
       <c r="K14" s="28"/>
       <c r="L14" s="28"/>
       <c r="M14" s="28"/>
-      <c r="N14" s="66"/>
-      <c r="O14" s="67"/>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B15" s="63"/>
-      <c r="C15" s="92"/>
+      <c r="N14" s="70"/>
+      <c r="O14" s="71"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B15" s="80"/>
+      <c r="C15" s="85"/>
       <c r="D15" s="2" t="s">
         <v>105</v>
       </c>
@@ -2928,12 +2949,12 @@
       <c r="K15" s="28"/>
       <c r="L15" s="28"/>
       <c r="M15" s="28"/>
-      <c r="N15" s="66"/>
-      <c r="O15" s="67"/>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B16" s="63"/>
-      <c r="C16" s="92"/>
+      <c r="N15" s="70"/>
+      <c r="O15" s="71"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B16" s="80"/>
+      <c r="C16" s="85"/>
       <c r="D16" s="2" t="s">
         <v>108</v>
       </c>
@@ -2946,12 +2967,12 @@
       <c r="K16" s="28"/>
       <c r="L16" s="28"/>
       <c r="M16" s="28"/>
-      <c r="N16" s="66"/>
-      <c r="O16" s="67"/>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B17" s="63"/>
-      <c r="C17" s="92"/>
+      <c r="N16" s="70"/>
+      <c r="O16" s="71"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B17" s="80"/>
+      <c r="C17" s="85"/>
       <c r="D17" s="2" t="s">
         <v>109</v>
       </c>
@@ -2964,12 +2985,12 @@
       <c r="K17" s="28"/>
       <c r="L17" s="28"/>
       <c r="M17" s="28"/>
-      <c r="N17" s="66"/>
-      <c r="O17" s="67"/>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B18" s="62"/>
-      <c r="C18" s="93"/>
+      <c r="N17" s="70"/>
+      <c r="O17" s="71"/>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B18" s="81"/>
+      <c r="C18" s="86"/>
       <c r="D18" s="2" t="s">
         <v>110</v>
       </c>
@@ -2982,14 +3003,14 @@
       <c r="K18" s="28"/>
       <c r="L18" s="28"/>
       <c r="M18" s="28"/>
-      <c r="N18" s="66"/>
-      <c r="O18" s="67"/>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B19" s="61">
+      <c r="N18" s="70"/>
+      <c r="O18" s="71"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B19" s="79">
         <v>3</v>
       </c>
-      <c r="C19" s="91"/>
+      <c r="C19" s="84"/>
       <c r="D19" s="2"/>
       <c r="G19" s="17">
         <v>12</v>
@@ -3000,12 +3021,12 @@
       <c r="K19" s="28"/>
       <c r="L19" s="28"/>
       <c r="M19" s="28"/>
-      <c r="N19" s="66"/>
-      <c r="O19" s="67"/>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B20" s="63"/>
-      <c r="C20" s="92"/>
+      <c r="N19" s="70"/>
+      <c r="O19" s="71"/>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B20" s="80"/>
+      <c r="C20" s="85"/>
       <c r="D20" s="2"/>
       <c r="G20" s="17">
         <v>13</v>
@@ -3016,12 +3037,12 @@
       <c r="K20" s="28"/>
       <c r="L20" s="28"/>
       <c r="M20" s="28"/>
-      <c r="N20" s="66"/>
-      <c r="O20" s="67"/>
-    </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B21" s="63"/>
-      <c r="C21" s="92"/>
+      <c r="N20" s="70"/>
+      <c r="O20" s="71"/>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B21" s="80"/>
+      <c r="C21" s="85"/>
       <c r="D21" s="2"/>
       <c r="G21" s="17">
         <v>14</v>
@@ -3032,12 +3053,12 @@
       <c r="K21" s="28"/>
       <c r="L21" s="28"/>
       <c r="M21" s="28"/>
-      <c r="N21" s="66"/>
-      <c r="O21" s="67"/>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B22" s="63"/>
-      <c r="C22" s="92"/>
+      <c r="N21" s="70"/>
+      <c r="O21" s="71"/>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B22" s="80"/>
+      <c r="C22" s="85"/>
       <c r="D22" s="2"/>
       <c r="G22" s="17">
         <v>15</v>
@@ -3048,12 +3069,12 @@
       <c r="K22" s="28"/>
       <c r="L22" s="28"/>
       <c r="M22" s="28"/>
-      <c r="N22" s="66"/>
-      <c r="O22" s="67"/>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B23" s="63"/>
-      <c r="C23" s="92"/>
+      <c r="N22" s="70"/>
+      <c r="O22" s="71"/>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B23" s="80"/>
+      <c r="C23" s="85"/>
       <c r="D23" s="2"/>
       <c r="G23" s="17">
         <v>16</v>
@@ -3064,12 +3085,12 @@
       <c r="K23" s="28"/>
       <c r="L23" s="28"/>
       <c r="M23" s="28"/>
-      <c r="N23" s="66"/>
-      <c r="O23" s="67"/>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B24" s="62"/>
-      <c r="C24" s="93"/>
+      <c r="N23" s="70"/>
+      <c r="O23" s="71"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B24" s="81"/>
+      <c r="C24" s="86"/>
       <c r="D24" s="2"/>
       <c r="G24" s="17">
         <v>17</v>
@@ -3080,14 +3101,14 @@
       <c r="K24" s="28"/>
       <c r="L24" s="28"/>
       <c r="M24" s="28"/>
-      <c r="N24" s="66"/>
-      <c r="O24" s="67"/>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B25" s="61">
+      <c r="N24" s="70"/>
+      <c r="O24" s="71"/>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B25" s="79">
         <v>4</v>
       </c>
-      <c r="C25" s="91"/>
+      <c r="C25" s="84"/>
       <c r="D25" s="2"/>
       <c r="G25" s="17">
         <v>18</v>
@@ -3098,48 +3119,72 @@
       <c r="K25" s="28"/>
       <c r="L25" s="28"/>
       <c r="M25" s="28"/>
-      <c r="N25" s="66"/>
-      <c r="O25" s="67"/>
-    </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B26" s="63"/>
-      <c r="C26" s="92"/>
+      <c r="N25" s="70"/>
+      <c r="O25" s="71"/>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B26" s="80"/>
+      <c r="C26" s="85"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B27" s="63"/>
-      <c r="C27" s="92"/>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B27" s="80"/>
+      <c r="C27" s="85"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B28" s="63"/>
-      <c r="C28" s="92"/>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B28" s="80"/>
+      <c r="C28" s="85"/>
       <c r="D28" s="2"/>
-      <c r="G28" s="75"/>
-      <c r="H28" s="75"/>
-      <c r="I28" s="88"/>
-      <c r="J28" s="88"/>
-      <c r="K28" s="88"/>
-      <c r="L28" s="88"/>
-      <c r="M28" s="88"/>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B29" s="63"/>
-      <c r="C29" s="92"/>
+      <c r="G28" s="64"/>
+      <c r="H28" s="64"/>
+      <c r="I28" s="94"/>
+      <c r="J28" s="94"/>
+      <c r="K28" s="94"/>
+      <c r="L28" s="94"/>
+      <c r="M28" s="94"/>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B29" s="80"/>
+      <c r="C29" s="85"/>
       <c r="D29" s="2"/>
-      <c r="I29" s="94"/>
-      <c r="J29" s="94"/>
-      <c r="K29" s="94"/>
-      <c r="L29" s="94"/>
-      <c r="M29" s="94"/>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B30" s="62"/>
-      <c r="C30" s="93"/>
+      <c r="I29" s="87"/>
+      <c r="J29" s="87"/>
+      <c r="K29" s="87"/>
+      <c r="L29" s="87"/>
+      <c r="M29" s="87"/>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B30" s="81"/>
+      <c r="C30" s="86"/>
       <c r="D30" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:M28"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="C19:C24"/>
+    <mergeCell ref="B19:B24"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="K6:M6"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="I6:I7"/>
@@ -3156,30 +3201,6 @@
     <mergeCell ref="N7:O7"/>
     <mergeCell ref="N8:O8"/>
     <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="C19:C24"/>
-    <mergeCell ref="B19:B24"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:M28"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="N21:O21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3194,20 +3215,20 @@
   </sheetPr>
   <dimension ref="B1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" customWidth="1"/>
+    <col min="6" max="6" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.53125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.53125" customWidth="1"/>
     <col min="9" max="9" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.77734375" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B1" s="57" t="s">
         <v>64</v>
       </c>
@@ -3215,47 +3236,47 @@
       <c r="D1" s="58"/>
       <c r="E1" s="59"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="111" t="s">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B3" s="98" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="111"/>
-      <c r="D3" s="111"/>
-      <c r="E3" s="111"/>
-      <c r="F3" s="111"/>
-      <c r="G3" s="111"/>
-      <c r="H3" s="111"/>
-      <c r="I3" s="111"/>
-      <c r="J3" s="111"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="72" t="s">
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B4" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="115" t="s">
+      <c r="C4" s="96" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="105" t="s">
+      <c r="D4" s="104" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="78" t="s">
+      <c r="E4" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="70" t="s">
+      <c r="F4" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="80" t="s">
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="80"/>
-    </row>
-    <row r="5" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="104"/>
-      <c r="C5" s="116"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="114"/>
+      <c r="J4" s="69"/>
+    </row>
+    <row r="5" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B5" s="103"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="95"/>
       <c r="F5" s="20" t="s">
         <v>86</v>
       </c>
@@ -3272,11 +3293,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="B6" s="18">
         <v>1</v>
       </c>
-      <c r="C6" s="102" t="s">
+      <c r="C6" s="115" t="s">
         <v>52</v>
       </c>
       <c r="D6" s="24" t="s">
@@ -3298,15 +3319,15 @@
         <v>89</v>
       </c>
       <c r="J6" s="18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B7" s="9">
         <f>B6+1</f>
         <v>2</v>
       </c>
-      <c r="C7" s="102"/>
+      <c r="C7" s="115"/>
       <c r="D7" s="25" t="s">
         <v>116</v>
       </c>
@@ -3326,15 +3347,15 @@
         <v>120</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B8" s="9">
         <f t="shared" ref="B8:B13" si="0">B7+1</f>
         <v>3</v>
       </c>
-      <c r="C8" s="102"/>
+      <c r="C8" s="115"/>
       <c r="D8" s="25" t="s">
         <v>48</v>
       </c>
@@ -3354,15 +3375,15 @@
         <v>121</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B9" s="9">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C9" s="102"/>
+      <c r="C9" s="115"/>
       <c r="D9" s="25" t="s">
         <v>117</v>
       </c>
@@ -3382,15 +3403,15 @@
         <v>120</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B10" s="9">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C10" s="102"/>
+      <c r="C10" s="115"/>
       <c r="D10" s="25"/>
       <c r="E10" s="9" t="s">
         <v>27</v>
@@ -3408,29 +3429,41 @@
         <v>89</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B11" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C11" s="102"/>
+      <c r="C11" s="115"/>
       <c r="D11" s="25"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="9"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E11" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="F11" s="117">
+        <v>1000</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="H11" s="8">
+        <v>10</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B12" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C12" s="102"/>
+      <c r="C12" s="115"/>
       <c r="D12" s="25"/>
       <c r="E12" s="9"/>
       <c r="F12" s="10"/>
@@ -3439,12 +3472,12 @@
       <c r="I12" s="5"/>
       <c r="J12" s="9"/>
     </row>
-    <row r="13" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B13" s="19">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C13" s="103"/>
+      <c r="C13" s="116"/>
       <c r="D13" s="26"/>
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
@@ -3453,7 +3486,7 @@
       <c r="I13" s="19"/>
       <c r="J13" s="19"/>
     </row>
-    <row r="14" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
       <c r="D14" s="22"/>
@@ -3466,7 +3499,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B15" s="21" t="s">
         <v>29</v>
       </c>
@@ -3478,112 +3511,116 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="2:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="98" t="s">
+    <row r="17" spans="2:12" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="C17" s="108" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="100"/>
-      <c r="E17" s="100"/>
-      <c r="F17" s="101"/>
+      <c r="D17" s="109"/>
+      <c r="E17" s="109"/>
+      <c r="F17" s="110"/>
       <c r="G17" s="32" t="s">
         <v>34</v>
       </c>
       <c r="H17" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="I17" s="98" t="s">
+      <c r="I17" s="108" t="s">
         <v>37</v>
       </c>
-      <c r="J17" s="99"/>
-      <c r="K17" s="100"/>
-      <c r="L17" s="101"/>
-    </row>
-    <row r="18" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="112" t="s">
+      <c r="J17" s="114"/>
+      <c r="K17" s="109"/>
+      <c r="L17" s="110"/>
+    </row>
+    <row r="18" spans="2:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B18" s="99" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="113" t="s">
+      <c r="C18" s="100" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="96" t="s">
+      <c r="D18" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="96" t="s">
+      <c r="E18" s="101" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="97" t="s">
+      <c r="F18" s="102" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="95" t="s">
+      <c r="G18" s="113" t="s">
         <v>53</v>
       </c>
-      <c r="H18" s="109" t="s">
+      <c r="H18" s="111" t="s">
         <v>30</v>
       </c>
-      <c r="I18" s="107" t="s">
+      <c r="I18" s="106" t="s">
         <v>30</v>
       </c>
-      <c r="J18" s="96" t="s">
+      <c r="J18" s="101" t="s">
         <v>42</v>
       </c>
-      <c r="K18" s="96" t="s">
+      <c r="K18" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="L18" s="97" t="s">
+      <c r="L18" s="102" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B19" s="112"/>
-      <c r="C19" s="113"/>
-      <c r="D19" s="96"/>
-      <c r="E19" s="96"/>
-      <c r="F19" s="97"/>
-      <c r="G19" s="95"/>
-      <c r="H19" s="110"/>
-      <c r="I19" s="108"/>
-      <c r="J19" s="96"/>
-      <c r="K19" s="96"/>
-      <c r="L19" s="97"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B19" s="99"/>
+      <c r="C19" s="100"/>
+      <c r="D19" s="101"/>
+      <c r="E19" s="101"/>
+      <c r="F19" s="102"/>
+      <c r="G19" s="113"/>
+      <c r="H19" s="112"/>
+      <c r="I19" s="107"/>
+      <c r="J19" s="101"/>
+      <c r="K19" s="101"/>
+      <c r="L19" s="102"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B20" s="35" t="s">
         <v>52</v>
       </c>
       <c r="C20" s="31">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D20" s="33">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E20" s="33">
         <v>3</v>
       </c>
-      <c r="F20" s="34"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="49" t="s">
-        <v>31</v>
+      <c r="F20" s="34">
+        <v>3</v>
+      </c>
+      <c r="G20" s="37">
+        <v>3</v>
+      </c>
+      <c r="H20" s="49">
+        <v>3</v>
       </c>
       <c r="I20" s="36" t="s">
         <v>31</v>
       </c>
       <c r="J20" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K20" s="33">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L20" s="34">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.45">
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.45">
       <c r="H22" t="s">
         <v>68</v>
       </c>
@@ -3593,28 +3630,28 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="I17:L17"/>
+    <mergeCell ref="C6:C13"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="D4:D5"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="I17:L17"/>
-    <mergeCell ref="C6:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3632,12 +3669,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D554F47F16D1AE46AF74397CE0A37779" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="24441d7a3758428b2811889d7d94fa0f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="28a9ec7f-d5a2-44c1-9222-13672e632811" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c373de015648521c434ab6f3362511f8" ns2:_="">
     <xsd:import namespace="28a9ec7f-d5a2-44c1-9222-13672e632811"/>
@@ -3775,6 +3806,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE7D9D9E-6447-4BB8-AD3E-F6023F68C701}">
   <ds:schemaRefs>
@@ -3784,15 +3821,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CBF06D4-65F6-44E9-92E0-EF775F2F24BD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1ACC35A4-912A-4C5D-808F-FA18702F7CFA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3808,4 +3836,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CBF06D4-65F6-44E9-92E0-EF775F2F24BD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added excel for WBT
</commit_message>
<xml_diff>
--- a/Docs/Lab2/Lab02_BBT_TCs_Form.xlsx
+++ b/Docs/Lab2/Lab02_BBT_TCs_Form.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B89F65-3783-417E-B782-875952DD7F93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51B82FD-ECBD-4752-A83F-90F5C080A4AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1460,6 +1460,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1475,8 +1478,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1496,176 +1547,125 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2011,7 +2011,7 @@
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2024,12 +2024,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10">
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="59"/>
       <c r="H1" s="42" t="s">
         <v>42</v>
       </c>
@@ -2037,11 +2037,11 @@
       <c r="J1" s="42"/>
     </row>
     <row r="2" spans="2:10">
-      <c r="H2" s="59" t="s">
+      <c r="H2" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
     </row>
     <row r="3" spans="2:10">
       <c r="H3" s="2"/>
@@ -2158,7 +2158,7 @@
       <c r="C20" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="H20" s="116"/>
+      <c r="H20" s="55"/>
     </row>
     <row r="21" spans="1:15">
       <c r="B21" s="1" t="s">
@@ -2201,21 +2201,21 @@
     </row>
     <row r="24" spans="1:15" ht="14.45" customHeight="1">
       <c r="A24" s="39"/>
-      <c r="B24" s="55" t="s">
+      <c r="B24" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="55"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="55"/>
-      <c r="I24" s="55"/>
-      <c r="J24" s="55"/>
-      <c r="K24" s="55"/>
-      <c r="L24" s="55"/>
-      <c r="M24" s="55"/>
-      <c r="N24" s="55"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="56"/>
+      <c r="I24" s="56"/>
+      <c r="J24" s="56"/>
+      <c r="K24" s="56"/>
+      <c r="L24" s="56"/>
+      <c r="M24" s="56"/>
+      <c r="N24" s="56"/>
     </row>
     <row r="26" spans="1:15">
       <c r="C26" s="41"/>
@@ -2258,39 +2258,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13">
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="59"/>
     </row>
     <row r="3" spans="2:13">
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="71"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="63"/>
     </row>
     <row r="5" spans="2:13">
-      <c r="B5" s="78" t="s">
+      <c r="B5" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="G5" s="79" t="s">
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="G5" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="79"/>
-      <c r="I5" s="79"/>
-      <c r="J5" s="79"/>
-      <c r="K5" s="79"/>
-      <c r="L5" s="79"/>
-      <c r="M5" s="79"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="73"/>
+      <c r="L5" s="73"/>
+      <c r="M5" s="73"/>
     </row>
     <row r="6" spans="2:13">
       <c r="B6" s="17" t="s">
@@ -2305,35 +2305,35 @@
       <c r="E6" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="81" t="s">
+      <c r="G6" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="75" t="s">
+      <c r="H6" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="60" t="s">
+      <c r="I6" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="80"/>
-      <c r="K6" s="80"/>
-      <c r="L6" s="77" t="s">
+      <c r="J6" s="75"/>
+      <c r="K6" s="75"/>
+      <c r="L6" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="77"/>
+      <c r="M6" s="69"/>
     </row>
     <row r="7" spans="2:13">
       <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C7" s="62" t="s">
+      <c r="C7" s="79" t="s">
         <v>69</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>69</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="76"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="68"/>
       <c r="I7" s="17" t="s">
         <v>82</v>
       </c>
@@ -2343,16 +2343,16 @@
       <c r="K7" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="L7" s="60" t="s">
+      <c r="L7" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="M7" s="61"/>
+      <c r="M7" s="78"/>
     </row>
     <row r="8" spans="2:13">
       <c r="B8" s="4">
         <v>2</v>
       </c>
-      <c r="C8" s="64"/>
+      <c r="C8" s="81"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
         <v>70</v>
@@ -2372,16 +2372,16 @@
       <c r="K8" s="2">
         <v>1</v>
       </c>
-      <c r="L8" s="73" t="s">
+      <c r="L8" s="65" t="s">
         <v>85</v>
       </c>
-      <c r="M8" s="74"/>
+      <c r="M8" s="66"/>
     </row>
     <row r="9" spans="2:13">
       <c r="B9" s="4">
         <v>3</v>
       </c>
-      <c r="C9" s="62" t="s">
+      <c r="C9" s="79" t="s">
         <v>80</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -2403,16 +2403,16 @@
       <c r="K9" s="2">
         <v>2.5</v>
       </c>
-      <c r="L9" s="73" t="s">
+      <c r="L9" s="65" t="s">
         <v>88</v>
       </c>
-      <c r="M9" s="74"/>
+      <c r="M9" s="66"/>
     </row>
     <row r="10" spans="2:13">
       <c r="B10" s="4">
         <v>4</v>
       </c>
-      <c r="C10" s="63"/>
+      <c r="C10" s="80"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
         <v>71</v>
@@ -2441,7 +2441,7 @@
       <c r="B11" s="4">
         <v>5</v>
       </c>
-      <c r="C11" s="64"/>
+      <c r="C11" s="81"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
         <v>72</v>
@@ -2461,16 +2461,16 @@
       <c r="K11" s="28">
         <v>10.35</v>
       </c>
-      <c r="L11" s="67" t="s">
+      <c r="L11" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="M11" s="68"/>
+      <c r="M11" s="71"/>
     </row>
     <row r="12" spans="2:13" ht="15" customHeight="1">
       <c r="B12" s="4">
         <v>6</v>
       </c>
-      <c r="C12" s="62" t="s">
+      <c r="C12" s="79" t="s">
         <v>74</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -2482,14 +2482,14 @@
       <c r="I12" s="28"/>
       <c r="J12" s="28"/>
       <c r="K12" s="28"/>
-      <c r="L12" s="67"/>
-      <c r="M12" s="68"/>
+      <c r="L12" s="70"/>
+      <c r="M12" s="71"/>
     </row>
     <row r="13" spans="2:13" ht="15" customHeight="1">
       <c r="B13" s="4">
         <v>7</v>
       </c>
-      <c r="C13" s="63"/>
+      <c r="C13" s="80"/>
       <c r="D13" s="4" t="s">
         <v>76</v>
       </c>
@@ -2506,7 +2506,7 @@
       <c r="B14" s="4">
         <v>8</v>
       </c>
-      <c r="C14" s="64"/>
+      <c r="C14" s="81"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
         <v>77</v>
@@ -2516,14 +2516,14 @@
       <c r="I14" s="28"/>
       <c r="J14" s="28"/>
       <c r="K14" s="28"/>
-      <c r="L14" s="67"/>
-      <c r="M14" s="68"/>
+      <c r="L14" s="70"/>
+      <c r="M14" s="71"/>
     </row>
     <row r="15" spans="2:13">
       <c r="B15" s="4">
         <v>9</v>
       </c>
-      <c r="C15" s="62" t="s">
+      <c r="C15" s="79" t="s">
         <v>78</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -2535,14 +2535,14 @@
       <c r="I15" s="28"/>
       <c r="J15" s="28"/>
       <c r="K15" s="28"/>
-      <c r="L15" s="67"/>
-      <c r="M15" s="68"/>
+      <c r="L15" s="70"/>
+      <c r="M15" s="71"/>
     </row>
     <row r="16" spans="2:13">
       <c r="B16" s="4">
         <v>10</v>
       </c>
-      <c r="C16" s="64"/>
+      <c r="C16" s="81"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
         <v>79</v>
@@ -2552,14 +2552,14 @@
       <c r="I16" s="28"/>
       <c r="J16" s="28"/>
       <c r="K16" s="28"/>
-      <c r="L16" s="67"/>
-      <c r="M16" s="68"/>
+      <c r="L16" s="70"/>
+      <c r="M16" s="71"/>
     </row>
     <row r="17" spans="2:13">
       <c r="B17" s="4">
         <v>11</v>
       </c>
-      <c r="C17" s="62" t="s">
+      <c r="C17" s="79" t="s">
         <v>93</v>
       </c>
       <c r="D17" s="4" t="s">
@@ -2571,14 +2571,14 @@
       <c r="I17" s="28"/>
       <c r="J17" s="28"/>
       <c r="K17" s="28"/>
-      <c r="L17" s="67"/>
-      <c r="M17" s="68"/>
+      <c r="L17" s="70"/>
+      <c r="M17" s="71"/>
     </row>
     <row r="18" spans="2:13">
       <c r="B18" s="4">
         <v>12</v>
       </c>
-      <c r="C18" s="64"/>
+      <c r="C18" s="81"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4" t="s">
         <v>81</v>
@@ -2588,14 +2588,14 @@
       <c r="I18" s="28"/>
       <c r="J18" s="28"/>
       <c r="K18" s="28"/>
-      <c r="L18" s="67"/>
-      <c r="M18" s="68"/>
+      <c r="L18" s="70"/>
+      <c r="M18" s="71"/>
     </row>
     <row r="19" spans="2:13">
       <c r="B19" s="4">
         <v>13</v>
       </c>
-      <c r="C19" s="62" t="s">
+      <c r="C19" s="79" t="s">
         <v>4</v>
       </c>
       <c r="D19" s="4"/>
@@ -2605,14 +2605,14 @@
       <c r="I19" s="28"/>
       <c r="J19" s="28"/>
       <c r="K19" s="28"/>
-      <c r="L19" s="67"/>
-      <c r="M19" s="68"/>
+      <c r="L19" s="70"/>
+      <c r="M19" s="71"/>
     </row>
     <row r="20" spans="2:13">
       <c r="B20" s="4">
         <v>14</v>
       </c>
-      <c r="C20" s="64"/>
+      <c r="C20" s="81"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="G20" s="48"/>
@@ -2620,14 +2620,14 @@
       <c r="I20" s="28"/>
       <c r="J20" s="28"/>
       <c r="K20" s="28"/>
-      <c r="L20" s="67"/>
-      <c r="M20" s="68"/>
+      <c r="L20" s="70"/>
+      <c r="M20" s="71"/>
     </row>
     <row r="21" spans="2:13">
       <c r="B21" s="4">
         <v>15</v>
       </c>
-      <c r="C21" s="62" t="s">
+      <c r="C21" s="79" t="s">
         <v>4</v>
       </c>
       <c r="D21" s="4"/>
@@ -2637,14 +2637,14 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
-      <c r="L21" s="65"/>
-      <c r="M21" s="66"/>
+      <c r="L21" s="82"/>
+      <c r="M21" s="83"/>
     </row>
     <row r="22" spans="2:13">
       <c r="B22" s="4">
         <v>16</v>
       </c>
-      <c r="C22" s="64"/>
+      <c r="C22" s="81"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
@@ -2657,11 +2657,24 @@
       <c r="D24" t="s">
         <v>21</v>
       </c>
-      <c r="F24" s="72"/>
-      <c r="G24" s="72"/>
+      <c r="F24" s="64"/>
+      <c r="G24" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C12:C14"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="F24:G24"/>
@@ -2678,19 +2691,6 @@
     <mergeCell ref="G5:M5"/>
     <mergeCell ref="I6:K6"/>
     <mergeCell ref="G6:G7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C12:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2726,41 +2726,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16">
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="59"/>
     </row>
     <row r="3" spans="2:16">
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="61" t="s">
         <v>118</v>
       </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="71"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="63"/>
     </row>
     <row r="5" spans="2:16">
-      <c r="B5" s="89" t="s">
+      <c r="B5" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
       <c r="E5" s="3"/>
-      <c r="G5" s="79" t="s">
+      <c r="G5" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="79"/>
-      <c r="I5" s="79"/>
-      <c r="J5" s="79"/>
-      <c r="K5" s="79"/>
-      <c r="L5" s="79"/>
-      <c r="M5" s="79"/>
-      <c r="N5" s="79"/>
-      <c r="O5" s="79"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="73"/>
+      <c r="L5" s="73"/>
+      <c r="M5" s="73"/>
+      <c r="N5" s="73"/>
+      <c r="O5" s="73"/>
     </row>
     <row r="6" spans="2:16" ht="14.45" customHeight="1">
       <c r="B6" s="4" t="s">
@@ -2773,30 +2773,30 @@
         <v>13</v>
       </c>
       <c r="E6" s="7"/>
-      <c r="G6" s="81" t="s">
+      <c r="G6" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="81" t="s">
+      <c r="H6" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="81" t="s">
+      <c r="I6" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="75" t="s">
+      <c r="J6" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="90" t="s">
+      <c r="K6" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="L6" s="92"/>
-      <c r="M6" s="92"/>
-      <c r="N6" s="90" t="s">
+      <c r="L6" s="93"/>
+      <c r="M6" s="93"/>
+      <c r="N6" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="O6" s="91"/>
+      <c r="O6" s="92"/>
     </row>
     <row r="7" spans="2:16">
-      <c r="B7" s="62">
+      <c r="B7" s="79">
         <v>1</v>
       </c>
       <c r="C7" s="84" t="s">
@@ -2805,10 +2805,10 @@
       <c r="D7" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="76"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="77"/>
+      <c r="J7" s="68"/>
       <c r="K7" s="17" t="s">
         <v>82</v>
       </c>
@@ -2818,13 +2818,13 @@
       <c r="M7" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="N7" s="60" t="s">
+      <c r="N7" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="O7" s="61"/>
+      <c r="O7" s="78"/>
     </row>
     <row r="8" spans="2:16">
-      <c r="B8" s="63"/>
+      <c r="B8" s="80"/>
       <c r="C8" s="85"/>
       <c r="D8" s="2" t="s">
         <v>96</v>
@@ -2844,14 +2844,14 @@
       <c r="K8" s="28"/>
       <c r="L8" s="28"/>
       <c r="M8" s="28"/>
-      <c r="N8" s="67"/>
-      <c r="O8" s="68"/>
+      <c r="N8" s="70"/>
+      <c r="O8" s="71"/>
       <c r="P8" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="9" spans="2:16">
-      <c r="B9" s="63"/>
+      <c r="B9" s="80"/>
       <c r="C9" s="85"/>
       <c r="D9" s="2" t="s">
         <v>97</v>
@@ -2871,13 +2871,13 @@
       <c r="K9" s="50"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
-      <c r="N9" s="87" t="s">
+      <c r="N9" s="88" t="s">
         <v>110</v>
       </c>
-      <c r="O9" s="88"/>
+      <c r="O9" s="89"/>
     </row>
     <row r="10" spans="2:16">
-      <c r="B10" s="63"/>
+      <c r="B10" s="80"/>
       <c r="C10" s="85"/>
       <c r="D10" s="2" t="s">
         <v>98</v>
@@ -2901,13 +2901,13 @@
       <c r="M10" s="28">
         <v>10</v>
       </c>
-      <c r="N10" s="67" t="s">
+      <c r="N10" s="70" t="s">
         <v>85</v>
       </c>
-      <c r="O10" s="68"/>
+      <c r="O10" s="71"/>
     </row>
     <row r="11" spans="2:16">
-      <c r="B11" s="63"/>
+      <c r="B11" s="80"/>
       <c r="C11" s="85"/>
       <c r="D11" s="2" t="s">
         <v>99</v>
@@ -2927,13 +2927,13 @@
       <c r="K11" s="27"/>
       <c r="L11" s="28"/>
       <c r="M11" s="28"/>
-      <c r="N11" s="87" t="s">
+      <c r="N11" s="88" t="s">
         <v>110</v>
       </c>
-      <c r="O11" s="68"/>
+      <c r="O11" s="71"/>
     </row>
     <row r="12" spans="2:16">
-      <c r="B12" s="64"/>
+      <c r="B12" s="81"/>
       <c r="C12" s="86"/>
       <c r="D12" s="2" t="s">
         <v>100</v>
@@ -2957,13 +2957,13 @@
       <c r="M12" s="28">
         <v>10</v>
       </c>
-      <c r="N12" s="67" t="s">
+      <c r="N12" s="70" t="s">
         <v>85</v>
       </c>
-      <c r="O12" s="68"/>
+      <c r="O12" s="71"/>
     </row>
     <row r="13" spans="2:16">
-      <c r="B13" s="62">
+      <c r="B13" s="79">
         <v>2</v>
       </c>
       <c r="C13" s="84" t="s">
@@ -2981,11 +2981,11 @@
       <c r="K13" s="16"/>
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
-      <c r="N13" s="87"/>
-      <c r="O13" s="88"/>
+      <c r="N13" s="88"/>
+      <c r="O13" s="89"/>
     </row>
     <row r="14" spans="2:16">
-      <c r="B14" s="63"/>
+      <c r="B14" s="80"/>
       <c r="C14" s="85"/>
       <c r="D14" s="2" t="s">
         <v>103</v>
@@ -2999,11 +2999,11 @@
       <c r="K14" s="28"/>
       <c r="L14" s="28"/>
       <c r="M14" s="28"/>
-      <c r="N14" s="67"/>
-      <c r="O14" s="68"/>
+      <c r="N14" s="70"/>
+      <c r="O14" s="71"/>
     </row>
     <row r="15" spans="2:16">
-      <c r="B15" s="63"/>
+      <c r="B15" s="80"/>
       <c r="C15" s="85"/>
       <c r="D15" s="2" t="s">
         <v>101</v>
@@ -3017,11 +3017,11 @@
       <c r="K15" s="28"/>
       <c r="L15" s="28"/>
       <c r="M15" s="28"/>
-      <c r="N15" s="67"/>
-      <c r="O15" s="68"/>
+      <c r="N15" s="70"/>
+      <c r="O15" s="71"/>
     </row>
     <row r="16" spans="2:16">
-      <c r="B16" s="63"/>
+      <c r="B16" s="80"/>
       <c r="C16" s="85"/>
       <c r="D16" s="2" t="s">
         <v>104</v>
@@ -3035,11 +3035,11 @@
       <c r="K16" s="28"/>
       <c r="L16" s="28"/>
       <c r="M16" s="28"/>
-      <c r="N16" s="67"/>
-      <c r="O16" s="68"/>
+      <c r="N16" s="70"/>
+      <c r="O16" s="71"/>
     </row>
     <row r="17" spans="2:15">
-      <c r="B17" s="63"/>
+      <c r="B17" s="80"/>
       <c r="C17" s="85"/>
       <c r="D17" s="2" t="s">
         <v>105</v>
@@ -3053,11 +3053,11 @@
       <c r="K17" s="28"/>
       <c r="L17" s="28"/>
       <c r="M17" s="28"/>
-      <c r="N17" s="67"/>
-      <c r="O17" s="68"/>
+      <c r="N17" s="70"/>
+      <c r="O17" s="71"/>
     </row>
     <row r="18" spans="2:15">
-      <c r="B18" s="64"/>
+      <c r="B18" s="81"/>
       <c r="C18" s="86"/>
       <c r="D18" s="2" t="s">
         <v>106</v>
@@ -3071,11 +3071,11 @@
       <c r="K18" s="28"/>
       <c r="L18" s="28"/>
       <c r="M18" s="28"/>
-      <c r="N18" s="67"/>
-      <c r="O18" s="68"/>
+      <c r="N18" s="70"/>
+      <c r="O18" s="71"/>
     </row>
     <row r="19" spans="2:15">
-      <c r="B19" s="62">
+      <c r="B19" s="79">
         <v>3</v>
       </c>
       <c r="C19" s="84"/>
@@ -3089,11 +3089,11 @@
       <c r="K19" s="28"/>
       <c r="L19" s="28"/>
       <c r="M19" s="28"/>
-      <c r="N19" s="67"/>
-      <c r="O19" s="68"/>
+      <c r="N19" s="70"/>
+      <c r="O19" s="71"/>
     </row>
     <row r="20" spans="2:15">
-      <c r="B20" s="63"/>
+      <c r="B20" s="80"/>
       <c r="C20" s="85"/>
       <c r="D20" s="2"/>
       <c r="G20" s="17">
@@ -3105,11 +3105,11 @@
       <c r="K20" s="28"/>
       <c r="L20" s="28"/>
       <c r="M20" s="28"/>
-      <c r="N20" s="67"/>
-      <c r="O20" s="68"/>
+      <c r="N20" s="70"/>
+      <c r="O20" s="71"/>
     </row>
     <row r="21" spans="2:15">
-      <c r="B21" s="63"/>
+      <c r="B21" s="80"/>
       <c r="C21" s="85"/>
       <c r="D21" s="2"/>
       <c r="G21" s="17">
@@ -3121,11 +3121,11 @@
       <c r="K21" s="28"/>
       <c r="L21" s="28"/>
       <c r="M21" s="28"/>
-      <c r="N21" s="67"/>
-      <c r="O21" s="68"/>
+      <c r="N21" s="70"/>
+      <c r="O21" s="71"/>
     </row>
     <row r="22" spans="2:15">
-      <c r="B22" s="63"/>
+      <c r="B22" s="80"/>
       <c r="C22" s="85"/>
       <c r="D22" s="2"/>
       <c r="G22" s="17">
@@ -3137,11 +3137,11 @@
       <c r="K22" s="28"/>
       <c r="L22" s="28"/>
       <c r="M22" s="28"/>
-      <c r="N22" s="67"/>
-      <c r="O22" s="68"/>
+      <c r="N22" s="70"/>
+      <c r="O22" s="71"/>
     </row>
     <row r="23" spans="2:15">
-      <c r="B23" s="63"/>
+      <c r="B23" s="80"/>
       <c r="C23" s="85"/>
       <c r="D23" s="2"/>
       <c r="G23" s="17">
@@ -3153,11 +3153,11 @@
       <c r="K23" s="28"/>
       <c r="L23" s="28"/>
       <c r="M23" s="28"/>
-      <c r="N23" s="67"/>
-      <c r="O23" s="68"/>
+      <c r="N23" s="70"/>
+      <c r="O23" s="71"/>
     </row>
     <row r="24" spans="2:15">
-      <c r="B24" s="64"/>
+      <c r="B24" s="81"/>
       <c r="C24" s="86"/>
       <c r="D24" s="2"/>
       <c r="G24" s="17">
@@ -3169,11 +3169,11 @@
       <c r="K24" s="28"/>
       <c r="L24" s="28"/>
       <c r="M24" s="28"/>
-      <c r="N24" s="67"/>
-      <c r="O24" s="68"/>
+      <c r="N24" s="70"/>
+      <c r="O24" s="71"/>
     </row>
     <row r="25" spans="2:15">
-      <c r="B25" s="62">
+      <c r="B25" s="79">
         <v>4</v>
       </c>
       <c r="C25" s="84"/>
@@ -3187,48 +3187,72 @@
       <c r="K25" s="28"/>
       <c r="L25" s="28"/>
       <c r="M25" s="28"/>
-      <c r="N25" s="67"/>
-      <c r="O25" s="68"/>
+      <c r="N25" s="70"/>
+      <c r="O25" s="71"/>
     </row>
     <row r="26" spans="2:15">
-      <c r="B26" s="63"/>
+      <c r="B26" s="80"/>
       <c r="C26" s="85"/>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="2:15">
-      <c r="B27" s="63"/>
+      <c r="B27" s="80"/>
       <c r="C27" s="85"/>
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="2:15">
-      <c r="B28" s="63"/>
+      <c r="B28" s="80"/>
       <c r="C28" s="85"/>
       <c r="D28" s="2"/>
-      <c r="G28" s="72"/>
-      <c r="H28" s="72"/>
-      <c r="I28" s="83"/>
-      <c r="J28" s="83"/>
-      <c r="K28" s="83"/>
-      <c r="L28" s="83"/>
-      <c r="M28" s="83"/>
+      <c r="G28" s="64"/>
+      <c r="H28" s="64"/>
+      <c r="I28" s="94"/>
+      <c r="J28" s="94"/>
+      <c r="K28" s="94"/>
+      <c r="L28" s="94"/>
+      <c r="M28" s="94"/>
     </row>
     <row r="29" spans="2:15">
-      <c r="B29" s="63"/>
+      <c r="B29" s="80"/>
       <c r="C29" s="85"/>
       <c r="D29" s="2"/>
-      <c r="I29" s="93"/>
-      <c r="J29" s="93"/>
-      <c r="K29" s="93"/>
-      <c r="L29" s="93"/>
-      <c r="M29" s="93"/>
+      <c r="I29" s="87"/>
+      <c r="J29" s="87"/>
+      <c r="K29" s="87"/>
+      <c r="L29" s="87"/>
+      <c r="M29" s="87"/>
     </row>
     <row r="30" spans="2:15">
-      <c r="B30" s="64"/>
+      <c r="B30" s="81"/>
       <c r="C30" s="86"/>
       <c r="D30" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:M28"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="C19:C24"/>
+    <mergeCell ref="B19:B24"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="K6:M6"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="I6:I7"/>
@@ -3245,30 +3269,6 @@
     <mergeCell ref="N7:O7"/>
     <mergeCell ref="N8:O8"/>
     <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="C19:C24"/>
-    <mergeCell ref="B19:B24"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:M28"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="N25:O25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3297,54 +3297,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10">
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="59"/>
     </row>
     <row r="3" spans="2:10">
-      <c r="B3" s="112" t="s">
+      <c r="B3" s="107" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="112"/>
-      <c r="G3" s="112"/>
-      <c r="H3" s="112"/>
-      <c r="I3" s="112"/>
-      <c r="J3" s="112"/>
+      <c r="C3" s="107"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="107"/>
+      <c r="F3" s="107"/>
+      <c r="G3" s="107"/>
+      <c r="H3" s="107"/>
+      <c r="I3" s="107"/>
+      <c r="J3" s="107"/>
     </row>
     <row r="4" spans="2:10">
-      <c r="B4" s="81" t="s">
+      <c r="B4" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="110" t="s">
+      <c r="C4" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="114" t="s">
+      <c r="D4" s="109" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="75" t="s">
+      <c r="E4" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="77" t="s">
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="77"/>
+      <c r="J4" s="69"/>
     </row>
     <row r="5" spans="2:10" ht="14.65" thickBot="1">
-      <c r="B5" s="113"/>
-      <c r="C5" s="111"/>
-      <c r="D5" s="115"/>
-      <c r="E5" s="109"/>
+      <c r="B5" s="108"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="110"/>
+      <c r="E5" s="104"/>
       <c r="F5" s="20" t="s">
         <v>82</v>
       </c>
@@ -3365,7 +3365,7 @@
       <c r="B6" s="18">
         <v>1</v>
       </c>
-      <c r="C6" s="100" t="s">
+      <c r="C6" s="114" t="s">
         <v>49</v>
       </c>
       <c r="D6" s="24" t="s">
@@ -3395,7 +3395,7 @@
         <f>B6+1</f>
         <v>2</v>
       </c>
-      <c r="C7" s="100"/>
+      <c r="C7" s="114"/>
       <c r="D7" s="25" t="s">
         <v>112</v>
       </c>
@@ -3423,7 +3423,7 @@
         <f t="shared" ref="B8:B13" si="0">B7+1</f>
         <v>3</v>
       </c>
-      <c r="C8" s="100"/>
+      <c r="C8" s="114"/>
       <c r="D8" s="25" t="s">
         <v>45</v>
       </c>
@@ -3451,7 +3451,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C9" s="100"/>
+      <c r="C9" s="114"/>
       <c r="D9" s="25" t="s">
         <v>113</v>
       </c>
@@ -3479,7 +3479,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C10" s="100"/>
+      <c r="C10" s="114"/>
       <c r="D10" s="25"/>
       <c r="E10" s="9" t="s">
         <v>27</v>
@@ -3505,7 +3505,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C11" s="100"/>
+      <c r="C11" s="114"/>
       <c r="D11" s="25"/>
       <c r="E11" s="9" t="s">
         <v>120</v>
@@ -3531,7 +3531,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C12" s="100"/>
+      <c r="C12" s="114"/>
       <c r="D12" s="25"/>
       <c r="E12" s="9"/>
       <c r="F12" s="10"/>
@@ -3545,7 +3545,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C13" s="101"/>
+      <c r="C13" s="115"/>
       <c r="D13" s="26"/>
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
@@ -3583,12 +3583,12 @@
       <c r="I16" s="6"/>
     </row>
     <row r="17" spans="2:16" ht="14.65" thickTop="1">
-      <c r="C17" s="96" t="s">
+      <c r="C17" s="97" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="98"/>
-      <c r="E17" s="98"/>
-      <c r="F17" s="99"/>
+      <c r="D17" s="99"/>
+      <c r="E17" s="99"/>
+      <c r="F17" s="100"/>
       <c r="G17" s="32" t="s">
         <v>33</v>
       </c>
@@ -3599,74 +3599,74 @@
       <c r="J17" s="118"/>
       <c r="K17" s="118"/>
       <c r="L17" s="119"/>
-      <c r="M17" s="96" t="s">
+      <c r="M17" s="97" t="s">
         <v>35</v>
       </c>
-      <c r="N17" s="97"/>
-      <c r="O17" s="98"/>
-      <c r="P17" s="99"/>
+      <c r="N17" s="98"/>
+      <c r="O17" s="99"/>
+      <c r="P17" s="100"/>
     </row>
     <row r="18" spans="2:16" ht="14.45" customHeight="1">
-      <c r="B18" s="107" t="s">
+      <c r="B18" s="111" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="108" t="s">
+      <c r="C18" s="112" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="94" t="s">
+      <c r="D18" s="113" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="94" t="s">
+      <c r="E18" s="113" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="95" t="s">
+      <c r="F18" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="G18" s="106" t="s">
+      <c r="G18" s="116" t="s">
         <v>50</v>
       </c>
-      <c r="H18" s="104" t="s">
+      <c r="H18" s="120" t="s">
         <v>30</v>
       </c>
-      <c r="I18" s="120"/>
-      <c r="J18" s="81" t="s">
+      <c r="I18" s="121"/>
+      <c r="J18" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="K18" s="81" t="s">
+      <c r="K18" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="L18" s="95" t="s">
+      <c r="L18" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="M18" s="102" t="s">
+      <c r="M18" s="101" t="s">
         <v>30</v>
       </c>
-      <c r="N18" s="81" t="s">
+      <c r="N18" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="O18" s="81" t="s">
+      <c r="O18" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="P18" s="95" t="s">
+      <c r="P18" s="103" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="19" spans="2:16">
-      <c r="B19" s="107"/>
-      <c r="C19" s="108"/>
-      <c r="D19" s="94"/>
-      <c r="E19" s="94"/>
-      <c r="F19" s="95"/>
-      <c r="G19" s="106"/>
-      <c r="H19" s="105"/>
-      <c r="I19" s="121"/>
-      <c r="J19" s="82"/>
-      <c r="K19" s="82"/>
-      <c r="L19" s="95"/>
-      <c r="M19" s="103"/>
-      <c r="N19" s="82"/>
-      <c r="O19" s="82"/>
-      <c r="P19" s="95"/>
+      <c r="B19" s="111"/>
+      <c r="C19" s="112"/>
+      <c r="D19" s="113"/>
+      <c r="E19" s="113"/>
+      <c r="F19" s="103"/>
+      <c r="G19" s="116"/>
+      <c r="H19" s="122"/>
+      <c r="I19" s="123"/>
+      <c r="J19" s="77"/>
+      <c r="K19" s="77"/>
+      <c r="L19" s="103"/>
+      <c r="M19" s="102"/>
+      <c r="N19" s="77"/>
+      <c r="O19" s="77"/>
+      <c r="P19" s="103"/>
     </row>
     <row r="20" spans="2:16">
       <c r="B20" s="35" t="s">
@@ -3687,10 +3687,10 @@
       <c r="G20" s="37">
         <v>3</v>
       </c>
-      <c r="H20" s="122" t="s">
+      <c r="H20" s="95" t="s">
         <v>109</v>
       </c>
-      <c r="I20" s="123"/>
+      <c r="I20" s="96"/>
       <c r="J20" s="2">
         <v>3</v>
       </c>
@@ -3726,12 +3726,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="M17:P17"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="P18:P19"/>
+    <mergeCell ref="C6:C13"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H17:L17"/>
+    <mergeCell ref="H18:I19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="F4:H4"/>
@@ -3740,19 +3745,14 @@
     <mergeCell ref="B3:J3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="D4:D5"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="M17:P17"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="P18:P19"/>
     <mergeCell ref="K18:K19"/>
     <mergeCell ref="L18:L19"/>
-    <mergeCell ref="C6:C13"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H17:L17"/>
-    <mergeCell ref="H18:I19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3761,6 +3761,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D554F47F16D1AE46AF74397CE0A37779" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="24441d7a3758428b2811889d7d94fa0f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="28a9ec7f-d5a2-44c1-9222-13672e632811" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c373de015648521c434ab6f3362511f8" ns2:_="">
     <xsd:import namespace="28a9ec7f-d5a2-44c1-9222-13672e632811"/>
@@ -3898,15 +3907,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3914,6 +3914,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE7D9D9E-6447-4BB8-AD3E-F6023F68C701}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1ACC35A4-912A-4C5D-808F-FA18702F7CFA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3931,14 +3939,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE7D9D9E-6447-4BB8-AD3E-F6023F68C701}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CBF06D4-65F6-44E9-92E0-EF775F2F24BD}">
   <ds:schemaRefs>

</xml_diff>